<commit_message>
add robust SE to table 4
</commit_message>
<xml_diff>
--- a/data/data_by_country.xlsx
+++ b/data/data_by_country.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilymickus/projectgit/CBD_research/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEFD452-1BE5-544D-A1FE-5AD56FE1F3FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BD52F8-6553-154C-985D-B3A0307DC25A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8059286A-9E56-C84F-897C-62ED17098FFF}"/>
+    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{8059286A-9E56-C84F-897C-62ED17098FFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2101,8 +2101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B688B4E9-7BE5-4346-80EE-CEFC8C089C55}">
   <dimension ref="A1:EB213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>